<commit_message>
Complete Phase 3: Unified CLI Application
- Created main.py to unify all functionality into a single command-line interface
- Implemented menu for inserting expenses, viewing visualizations, creating backups, and deleting data
- Refactored manual_backup.py and delete_data.py into callable functions
- Centralized saving and sorting logic into expense_utils.py (save_expense_entry)
- Cleaned imports and modularized project structure
- Restructured project folders into /app, /visuals, /tools, /data for better scalability
- Ensured all expense entries are automatically sorted by date upon saving
- Finalized and stabilized Phase 3 system ready for GUI development
</commit_message>
<xml_diff>
--- a/data/Expense_Tracker.xlsx
+++ b/data/Expense_Tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>191.02</v>
+        <v>75.81999999999999</v>
       </c>
       <c r="D63" t="inlineStr"/>
     </row>
@@ -1455,11 +1455,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>75.81999999999999</v>
+        <v>191.02</v>
       </c>
       <c r="D64" t="inlineStr"/>
     </row>
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>17.42</v>
+        <v>119.13</v>
       </c>
       <c r="D88" t="inlineStr"/>
     </row>
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>119.13</v>
+        <v>17.42</v>
       </c>
       <c r="D89" t="inlineStr"/>
     </row>
@@ -2031,11 +2031,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>80.29000000000001</v>
+        <v>52.66</v>
       </c>
       <c r="D100" t="inlineStr"/>
     </row>
@@ -2047,11 +2047,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>52.66</v>
+        <v>12.83</v>
       </c>
       <c r="D101" t="inlineStr"/>
     </row>
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>12.83</v>
+        <v>80.29000000000001</v>
       </c>
       <c r="D102" t="inlineStr"/>
     </row>
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>74.06999999999999</v>
+        <v>126.16</v>
       </c>
       <c r="D113" t="inlineStr"/>
     </row>
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>126.16</v>
+        <v>74.06999999999999</v>
       </c>
       <c r="D114" t="inlineStr"/>
     </row>
@@ -2447,11 +2447,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>158.48</v>
+        <v>127.43</v>
       </c>
       <c r="D126" t="inlineStr"/>
     </row>
@@ -2463,11 +2463,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>127.43</v>
+        <v>158.48</v>
       </c>
       <c r="D127" t="inlineStr"/>
     </row>
@@ -2623,11 +2623,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>146.69</v>
+        <v>21.48</v>
       </c>
       <c r="D137" t="inlineStr"/>
     </row>
@@ -2655,11 +2655,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>21.48</v>
+        <v>146.69</v>
       </c>
       <c r="D139" t="inlineStr"/>
     </row>
@@ -2815,11 +2815,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>125.39</v>
+        <v>101.09</v>
       </c>
       <c r="D149" t="inlineStr"/>
     </row>
@@ -2831,11 +2831,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>199</v>
+        <v>6.21</v>
       </c>
       <c r="D150" t="inlineStr"/>
     </row>
@@ -2847,11 +2847,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>6.21</v>
+        <v>199</v>
       </c>
       <c r="D151" t="inlineStr"/>
     </row>
@@ -2863,11 +2863,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>101.09</v>
+        <v>125.39</v>
       </c>
       <c r="D152" t="inlineStr"/>
     </row>
@@ -3023,11 +3023,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>105.4</v>
+        <v>177.11</v>
       </c>
       <c r="D162" t="inlineStr"/>
     </row>
@@ -3039,11 +3039,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>115.05</v>
+        <v>180.03</v>
       </c>
       <c r="D163" t="inlineStr"/>
     </row>
@@ -3055,11 +3055,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>159.19</v>
+        <v>115.05</v>
       </c>
       <c r="D164" t="inlineStr"/>
     </row>
@@ -3071,11 +3071,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>180.03</v>
+        <v>105.4</v>
       </c>
       <c r="D165" t="inlineStr"/>
     </row>
@@ -3087,11 +3087,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>177.11</v>
+        <v>159.19</v>
       </c>
       <c r="D166" t="inlineStr"/>
     </row>
@@ -3203,7 +3203,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>111.86</v>
+        <v>47.34</v>
       </c>
       <c r="D173" t="inlineStr"/>
     </row>
@@ -3219,7 +3219,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>47.34</v>
+        <v>111.86</v>
       </c>
       <c r="D174" t="inlineStr"/>
     </row>
@@ -3231,11 +3231,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>196.23</v>
+        <v>72.81</v>
       </c>
       <c r="D175" t="inlineStr"/>
     </row>
@@ -3247,11 +3247,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>72.81</v>
+        <v>196.23</v>
       </c>
       <c r="D176" t="inlineStr"/>
     </row>
@@ -3610,50 +3610,90 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025/04/29</t>
+          <t>2025/04/28</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>69.84999999999999</v>
-      </c>
-      <c r="D199" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025/04/30</t>
+          <t>2025/04/29</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>94.58</v>
+        <v>69.84999999999999</v>
       </c>
       <c r="D200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
+          <t>2025/04/29</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Restaurant</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>20</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
           <t>2025/04/30</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>94.58</v>
+      </c>
+      <c r="D202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025/04/30</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
         <is>
           <t>Shopping</t>
         </is>
       </c>
-      <c r="C201" t="n">
+      <c r="C203" t="n">
         <v>6.51</v>
       </c>
-      <c r="D201" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Complete Phase 4: GUI Integration and Polishing
- Developed full-featured GUI using Tkinter with 3-panel layout (Visualize, Insert, Tools)
- Connected all backend functionality (insert entry, backup, delete, visualizations)
- Made layout responsive and centered with dynamic sizing
- Applied visual refinements: input sizing, spacing, launch centering
- Implemented `.bat` launcher for quick startup (executable to be explored later)
</commit_message>
<xml_diff>
--- a/data/Expense_Tracker.xlsx
+++ b/data/Expense_Tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D203"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,11 +655,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>119.26</v>
+        <v>105.95</v>
       </c>
       <c r="D14" t="inlineStr"/>
     </row>
@@ -671,11 +671,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>105.95</v>
+        <v>89.78</v>
       </c>
       <c r="D15" t="inlineStr"/>
     </row>
@@ -687,11 +687,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>89.78</v>
+        <v>119.26</v>
       </c>
       <c r="D16" t="inlineStr"/>
     </row>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>177.51</v>
+        <v>169.37</v>
       </c>
       <c r="D52" t="inlineStr"/>
     </row>
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>169.37</v>
+        <v>177.51</v>
       </c>
       <c r="D53" t="inlineStr"/>
     </row>
@@ -1295,11 +1295,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42.06</v>
+        <v>91.19</v>
       </c>
       <c r="D54" t="inlineStr"/>
     </row>
@@ -1311,11 +1311,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>91.19</v>
+        <v>42.06</v>
       </c>
       <c r="D55" t="inlineStr"/>
     </row>
@@ -2671,11 +2671,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>45.66</v>
+        <v>21.07</v>
       </c>
       <c r="D140" t="inlineStr"/>
     </row>
@@ -2703,11 +2703,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>21.07</v>
+        <v>169.93</v>
       </c>
       <c r="D142" t="inlineStr"/>
     </row>
@@ -2735,11 +2735,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>169.93</v>
+        <v>45.66</v>
       </c>
       <c r="D144" t="inlineStr"/>
     </row>
@@ -2815,11 +2815,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>101.09</v>
+        <v>6.21</v>
       </c>
       <c r="D149" t="inlineStr"/>
     </row>
@@ -2831,11 +2831,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>6.21</v>
+        <v>199</v>
       </c>
       <c r="D150" t="inlineStr"/>
     </row>
@@ -2847,11 +2847,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>199</v>
+        <v>101.09</v>
       </c>
       <c r="D151" t="inlineStr"/>
     </row>
@@ -3023,11 +3023,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>177.11</v>
+        <v>180.03</v>
       </c>
       <c r="D162" t="inlineStr"/>
     </row>
@@ -3039,11 +3039,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>180.03</v>
+        <v>105.4</v>
       </c>
       <c r="D163" t="inlineStr"/>
     </row>
@@ -3055,11 +3055,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>115.05</v>
+        <v>177.11</v>
       </c>
       <c r="D164" t="inlineStr"/>
     </row>
@@ -3071,11 +3071,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>105.4</v>
+        <v>159.19</v>
       </c>
       <c r="D165" t="inlineStr"/>
     </row>
@@ -3087,11 +3087,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>159.19</v>
+        <v>115.05</v>
       </c>
       <c r="D166" t="inlineStr"/>
     </row>
@@ -3439,11 +3439,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>171.79</v>
+        <v>199.43</v>
       </c>
       <c r="D188" t="inlineStr"/>
     </row>
@@ -3455,11 +3455,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>183.49</v>
+        <v>171.79</v>
       </c>
       <c r="D189" t="inlineStr"/>
     </row>
@@ -3471,11 +3471,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>199.43</v>
+        <v>183.49</v>
       </c>
       <c r="D190" t="inlineStr"/>
     </row>
@@ -3659,41 +3659,81 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>test4</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025/04/30</t>
+          <t>2025/04/29</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>94.58</v>
-      </c>
-      <c r="D202" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
+          <t>2025/04/29</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Restaurant</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>20</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
           <t>2025/04/30</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr">
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>94.58</v>
+      </c>
+      <c r="D204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025/04/30</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
         <is>
           <t>Shopping</t>
         </is>
       </c>
-      <c r="C203" t="n">
+      <c r="C205" t="n">
         <v>6.51</v>
       </c>
-      <c r="D203" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Minor changes: - Made GUI more visually pleasing - Made .bat executable from anywhere
</commit_message>
<xml_diff>
--- a/data/Expense_Tracker.xlsx
+++ b/data/Expense_Tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,11 +655,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>119.26</v>
+        <v>89.78</v>
       </c>
       <c r="D14" t="inlineStr"/>
     </row>
@@ -671,11 +671,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>105.95</v>
+        <v>119.26</v>
       </c>
       <c r="D15" t="inlineStr"/>
     </row>
@@ -687,11 +687,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>89.78</v>
+        <v>105.95</v>
       </c>
       <c r="D16" t="inlineStr"/>
     </row>
@@ -863,11 +863,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>129.89</v>
+        <v>76.5</v>
       </c>
       <c r="D27" t="inlineStr"/>
     </row>
@@ -879,11 +879,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>76.5</v>
+        <v>129.89</v>
       </c>
       <c r="D28" t="inlineStr"/>
     </row>
@@ -1263,11 +1263,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>42.06</v>
+        <v>177.51</v>
       </c>
       <c r="D52" t="inlineStr"/>
     </row>
@@ -1279,11 +1279,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>91.19</v>
+        <v>169.37</v>
       </c>
       <c r="D53" t="inlineStr"/>
     </row>
@@ -1295,11 +1295,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>169.37</v>
+        <v>42.06</v>
       </c>
       <c r="D54" t="inlineStr"/>
     </row>
@@ -1311,11 +1311,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>177.51</v>
+        <v>91.19</v>
       </c>
       <c r="D55" t="inlineStr"/>
     </row>
@@ -1663,11 +1663,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>25.39</v>
+        <v>36.96</v>
       </c>
       <c r="D77" t="inlineStr"/>
     </row>
@@ -1679,11 +1679,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>36.96</v>
+        <v>25.39</v>
       </c>
       <c r="D78" t="inlineStr"/>
     </row>
@@ -1695,11 +1695,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>49.5</v>
+        <v>19.68</v>
       </c>
       <c r="D79" t="inlineStr"/>
     </row>
@@ -1711,11 +1711,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>40.23</v>
+        <v>49.5</v>
       </c>
       <c r="D80" t="inlineStr"/>
     </row>
@@ -1727,11 +1727,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>19.68</v>
+        <v>40.23</v>
       </c>
       <c r="D81" t="inlineStr"/>
     </row>
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>17.42</v>
+        <v>119.13</v>
       </c>
       <c r="D88" t="inlineStr"/>
     </row>
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>119.13</v>
+        <v>17.42</v>
       </c>
       <c r="D89" t="inlineStr"/>
     </row>
@@ -1871,11 +1871,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>50.47</v>
+        <v>71.19</v>
       </c>
       <c r="D90" t="inlineStr"/>
     </row>
@@ -1887,11 +1887,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>71.19</v>
+        <v>50.47</v>
       </c>
       <c r="D91" t="inlineStr"/>
     </row>
@@ -1999,11 +1999,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>28.46</v>
+        <v>182.12</v>
       </c>
       <c r="D98" t="inlineStr"/>
     </row>
@@ -2015,11 +2015,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>182.12</v>
+        <v>28.46</v>
       </c>
       <c r="D99" t="inlineStr"/>
     </row>
@@ -2031,11 +2031,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Snacks</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>12.83</v>
+        <v>80.29000000000001</v>
       </c>
       <c r="D100" t="inlineStr"/>
     </row>
@@ -2047,11 +2047,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>80.29000000000001</v>
+        <v>52.66</v>
       </c>
       <c r="D101" t="inlineStr"/>
     </row>
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Snacks</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>52.66</v>
+        <v>12.83</v>
       </c>
       <c r="D102" t="inlineStr"/>
     </row>
@@ -2495,11 +2495,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>62.92</v>
+        <v>75.84999999999999</v>
       </c>
       <c r="D129" t="inlineStr"/>
     </row>
@@ -2511,11 +2511,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>80.59</v>
+        <v>151.66</v>
       </c>
       <c r="D130" t="inlineStr"/>
     </row>
@@ -2527,11 +2527,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>151.66</v>
+        <v>80.59</v>
       </c>
       <c r="D131" t="inlineStr"/>
     </row>
@@ -2543,11 +2543,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>75.84999999999999</v>
+        <v>62.92</v>
       </c>
       <c r="D132" t="inlineStr"/>
     </row>
@@ -2671,11 +2671,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>62.67</v>
+        <v>83.48</v>
       </c>
       <c r="D140" t="inlineStr"/>
     </row>
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>45.66</v>
+        <v>169.93</v>
       </c>
       <c r="D141" t="inlineStr"/>
     </row>
@@ -2703,11 +2703,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>169.93</v>
+        <v>21.07</v>
       </c>
       <c r="D142" t="inlineStr"/>
     </row>
@@ -2719,11 +2719,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>83.48</v>
+        <v>62.67</v>
       </c>
       <c r="D143" t="inlineStr"/>
     </row>
@@ -2735,11 +2735,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>21.07</v>
+        <v>45.66</v>
       </c>
       <c r="D144" t="inlineStr"/>
     </row>
@@ -2927,11 +2927,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Laundry</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>34.21</v>
+        <v>121.27</v>
       </c>
       <c r="D156" t="inlineStr"/>
     </row>
@@ -2943,11 +2943,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>180.79</v>
+        <v>34.21</v>
       </c>
       <c r="D157" t="inlineStr"/>
     </row>
@@ -2959,11 +2959,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Laundry</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>121.27</v>
+        <v>180.79</v>
       </c>
       <c r="D158" t="inlineStr"/>
     </row>
@@ -3119,11 +3119,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>171.59</v>
+        <v>38.46</v>
       </c>
       <c r="D168" t="inlineStr"/>
     </row>
@@ -3135,11 +3135,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>38.46</v>
+        <v>12.48</v>
       </c>
       <c r="D169" t="inlineStr"/>
     </row>
@@ -3151,11 +3151,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>106.97</v>
+        <v>171.59</v>
       </c>
       <c r="D170" t="inlineStr"/>
     </row>
@@ -3167,11 +3167,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>12.48</v>
+        <v>106.97</v>
       </c>
       <c r="D171" t="inlineStr"/>
     </row>
@@ -3311,11 +3311,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>14.78</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="D180" t="inlineStr"/>
     </row>
@@ -3327,11 +3327,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>69.01000000000001</v>
+        <v>189.01</v>
       </c>
       <c r="D181" t="inlineStr"/>
     </row>
@@ -3343,11 +3343,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>189.01</v>
+        <v>14.78</v>
       </c>
       <c r="D182" t="inlineStr"/>
     </row>
@@ -3439,11 +3439,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>199.43</v>
+        <v>183.49</v>
       </c>
       <c r="D188" t="inlineStr"/>
     </row>
@@ -3455,11 +3455,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>171.79</v>
+        <v>199.43</v>
       </c>
       <c r="D189" t="inlineStr"/>
     </row>
@@ -3471,11 +3471,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>183.49</v>
+        <v>171.79</v>
       </c>
       <c r="D190" t="inlineStr"/>
     </row>
@@ -3487,11 +3487,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Toters</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>92.91</v>
+        <v>69.18000000000001</v>
       </c>
       <c r="D191" t="inlineStr"/>
     </row>
@@ -3503,11 +3503,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Toters</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>69.18000000000001</v>
+        <v>92.91</v>
       </c>
       <c r="D192" t="inlineStr"/>
     </row>
@@ -3635,13 +3635,17 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>69.84999999999999</v>
-      </c>
-      <c r="D200" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>test5</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -3659,7 +3663,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>test4</t>
+          <t>test3</t>
         </is>
       </c>
     </row>
@@ -3675,11 +3679,11 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>test6</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3703,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>test3</t>
+          <t>test4</t>
         </is>
       </c>
     </row>
@@ -3711,33 +3715,33 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Restaurant</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>20</v>
-      </c>
-      <c r="D204" t="inlineStr">
-        <is>
-          <t>test5</t>
-        </is>
-      </c>
+        <v>69.84999999999999</v>
+      </c>
+      <c r="D204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025/04/30</t>
+          <t>2025/04/29</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Restaurant</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>94.58</v>
-      </c>
-      <c r="D205" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -3747,13 +3751,29 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>94.58</v>
+      </c>
+      <c r="D206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025/04/30</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
           <t>Shopping</t>
         </is>
       </c>
-      <c r="C206" t="n">
+      <c r="C207" t="n">
         <v>6.51</v>
       </c>
-      <c r="D206" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>